<commit_message>
doc: 2019-12-24 공부한 내용 추가
</commit_message>
<xml_diff>
--- a/projects/ui_development/documents/2.테스트결과서_김현욱.xlsx
+++ b/projects/ui_development/documents/2.테스트결과서_김현욱.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="29040" windowHeight="16440" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="29040" windowHeight="16440" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="표지" sheetId="19" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="118">
   <si>
     <t>Step</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -485,6 +485,13 @@
   </si>
   <si>
     <t>[성별을 선택해주세요]라는 메시지 출력</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>O</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -621,7 +628,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="38">
+  <borders count="36">
     <border>
       <left/>
       <right/>
@@ -1086,32 +1093,6 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="dotted">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="dotted">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
       <bottom style="dotted">
         <color indexed="64"/>
       </bottom>
@@ -1145,7 +1126,7 @@
     <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="142">
+  <cellXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1210,16 +1191,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1259,77 +1231,62 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1349,16 +1306,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1379,26 +1327,65 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1421,62 +1408,32 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1493,37 +1450,31 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1541,31 +1492,22 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1889,130 +1831,130 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="30"/>
+      <c r="A1" s="27"/>
     </row>
     <row r="2" spans="1:1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="30"/>
+      <c r="A2" s="27"/>
     </row>
     <row r="3" spans="1:1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="30"/>
+      <c r="A3" s="27"/>
     </row>
     <row r="4" spans="1:1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="30"/>
+      <c r="A4" s="27"/>
     </row>
     <row r="5" spans="1:1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="30"/>
+      <c r="A5" s="27"/>
     </row>
     <row r="6" spans="1:1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="30"/>
+      <c r="A6" s="27"/>
     </row>
     <row r="7" spans="1:1" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="35"/>
+      <c r="A7" s="32"/>
     </row>
     <row r="8" spans="1:1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="30"/>
+      <c r="A8" s="27"/>
     </row>
     <row r="9" spans="1:1" ht="46.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="29" t="s">
+      <c r="A9" s="26" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="32"/>
+      <c r="A10" s="29"/>
     </row>
     <row r="11" spans="1:1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="31"/>
+      <c r="A11" s="28"/>
     </row>
     <row r="12" spans="1:1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="31"/>
+      <c r="A12" s="28"/>
     </row>
     <row r="13" spans="1:1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="31"/>
+      <c r="A13" s="28"/>
     </row>
     <row r="14" spans="1:1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="31"/>
+      <c r="A14" s="28"/>
     </row>
     <row r="15" spans="1:1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="31"/>
+      <c r="A15" s="28"/>
     </row>
     <row r="16" spans="1:1" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="32"/>
+      <c r="A16" s="29"/>
     </row>
     <row r="17" spans="1:1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="31"/>
+      <c r="A17" s="28"/>
     </row>
     <row r="18" spans="1:1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="31"/>
+      <c r="A18" s="28"/>
     </row>
     <row r="19" spans="1:1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="31"/>
+      <c r="A19" s="28"/>
     </row>
     <row r="20" spans="1:1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="31"/>
+      <c r="A20" s="28"/>
     </row>
     <row r="21" spans="1:1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="31"/>
+      <c r="A21" s="28"/>
     </row>
     <row r="22" spans="1:1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="31"/>
+      <c r="A22" s="28"/>
     </row>
     <row r="23" spans="1:1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="31"/>
+      <c r="A23" s="28"/>
     </row>
     <row r="24" spans="1:1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="31"/>
+      <c r="A24" s="28"/>
     </row>
     <row r="25" spans="1:1" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="36"/>
+      <c r="A25" s="33"/>
     </row>
     <row r="26" spans="1:1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="31"/>
+      <c r="A26" s="28"/>
     </row>
     <row r="27" spans="1:1" ht="27" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="37" t="s">
+      <c r="A27" s="34" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="28" spans="1:1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="30"/>
+      <c r="A28" s="27"/>
     </row>
     <row r="29" spans="1:1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="30"/>
+      <c r="A29" s="27"/>
     </row>
     <row r="30" spans="1:1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="30"/>
+      <c r="A30" s="27"/>
     </row>
     <row r="31" spans="1:1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="30"/>
+      <c r="A31" s="27"/>
     </row>
     <row r="32" spans="1:1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="30"/>
+      <c r="A32" s="27"/>
     </row>
     <row r="33" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="30"/>
+      <c r="A33" s="27"/>
     </row>
     <row r="34" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="30"/>
+      <c r="A34" s="27"/>
     </row>
     <row r="35" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="30"/>
+      <c r="A35" s="27"/>
     </row>
     <row r="36" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="30"/>
+      <c r="A36" s="27"/>
     </row>
     <row r="37" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A37" s="30"/>
+      <c r="A37" s="27"/>
     </row>
     <row r="38" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A38" s="30"/>
+      <c r="A38" s="27"/>
     </row>
     <row r="39" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A39" s="34"/>
-      <c r="B39" s="33"/>
+      <c r="A39" s="31"/>
+      <c r="B39" s="30"/>
     </row>
     <row r="40" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A40" s="34"/>
-      <c r="B40" s="33"/>
+      <c r="A40" s="31"/>
+      <c r="B40" s="30"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -2029,8 +1971,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2048,94 +1990,94 @@
   <sheetData>
     <row r="1" spans="1:10" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="86" t="s">
+      <c r="A2" s="88" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="87"/>
-      <c r="C2" s="88" t="s">
+      <c r="B2" s="89"/>
+      <c r="C2" s="90" t="s">
         <v>78</v>
       </c>
-      <c r="D2" s="88"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="88"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
       <c r="I2" s="14"/>
       <c r="J2" s="14"/>
     </row>
     <row r="3" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="89" t="s">
+      <c r="A3" s="91" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="90"/>
-      <c r="C3" s="91" t="s">
+      <c r="B3" s="92"/>
+      <c r="C3" s="93" t="s">
         <v>64</v>
       </c>
-      <c r="D3" s="91"/>
-      <c r="E3" s="91"/>
-      <c r="F3" s="91"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="93"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
       <c r="I3" s="14"/>
       <c r="J3" s="14"/>
     </row>
     <row r="4" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="89" t="s">
+      <c r="A4" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="90"/>
-      <c r="C4" s="92" t="s">
+      <c r="B4" s="92"/>
+      <c r="C4" s="94" t="s">
         <v>65</v>
       </c>
-      <c r="D4" s="92"/>
-      <c r="E4" s="92"/>
-      <c r="F4" s="92"/>
+      <c r="D4" s="94"/>
+      <c r="E4" s="94"/>
+      <c r="F4" s="94"/>
       <c r="G4" s="15"/>
       <c r="H4" s="15"/>
       <c r="I4" s="14"/>
       <c r="J4" s="14"/>
     </row>
     <row r="5" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="98" t="s">
+      <c r="A5" s="76" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="99"/>
-      <c r="C5" s="102" t="s">
+      <c r="B5" s="77"/>
+      <c r="C5" s="80" t="s">
         <v>66</v>
       </c>
-      <c r="D5" s="102"/>
-      <c r="E5" s="102"/>
-      <c r="F5" s="102"/>
+      <c r="D5" s="80"/>
+      <c r="E5" s="80"/>
+      <c r="F5" s="80"/>
       <c r="G5" s="16"/>
       <c r="H5" s="16"/>
       <c r="I5" s="14"/>
       <c r="J5" s="14"/>
     </row>
     <row r="6" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="100"/>
-      <c r="B6" s="101"/>
-      <c r="C6" s="103" t="s">
+      <c r="A6" s="78"/>
+      <c r="B6" s="79"/>
+      <c r="C6" s="81" t="s">
         <v>67</v>
       </c>
-      <c r="D6" s="103"/>
-      <c r="E6" s="103"/>
-      <c r="F6" s="103"/>
+      <c r="D6" s="81"/>
+      <c r="E6" s="81"/>
+      <c r="F6" s="81"/>
       <c r="G6" s="16"/>
       <c r="H6" s="16"/>
       <c r="I6" s="14"/>
       <c r="J6" s="14"/>
     </row>
     <row r="7" spans="1:10" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="104" t="s">
+      <c r="A7" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="105"/>
-      <c r="C7" s="106" t="s">
+      <c r="B7" s="83"/>
+      <c r="C7" s="84" t="s">
         <v>68</v>
       </c>
-      <c r="D7" s="106"/>
-      <c r="E7" s="106"/>
-      <c r="F7" s="106"/>
+      <c r="D7" s="84"/>
+      <c r="E7" s="84"/>
+      <c r="F7" s="84"/>
       <c r="G7" s="16"/>
       <c r="H7" s="16"/>
       <c r="I7" s="14"/>
@@ -2143,238 +2085,278 @@
     </row>
     <row r="8" spans="1:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="9" spans="1:10" s="19" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="107" t="s">
+      <c r="A9" s="85" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="108" t="s">
+      <c r="B9" s="86" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="94" t="s">
+      <c r="C9" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="94" t="s">
+      <c r="D9" s="72" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="94" t="s">
+      <c r="E9" s="72" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="94" t="s">
+      <c r="F9" s="72" t="s">
         <v>19</v>
       </c>
-      <c r="G9" s="94" t="s">
+      <c r="G9" s="72" t="s">
         <v>20</v>
       </c>
-      <c r="H9" s="96" t="s">
+      <c r="H9" s="74" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:10" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="100"/>
-      <c r="B10" s="109"/>
-      <c r="C10" s="95"/>
-      <c r="D10" s="95"/>
-      <c r="E10" s="95"/>
-      <c r="F10" s="95"/>
-      <c r="G10" s="95"/>
-      <c r="H10" s="97"/>
+      <c r="A10" s="78"/>
+      <c r="B10" s="87"/>
+      <c r="C10" s="73"/>
+      <c r="D10" s="73"/>
+      <c r="E10" s="73"/>
+      <c r="F10" s="73"/>
+      <c r="G10" s="73"/>
+      <c r="H10" s="75"/>
     </row>
     <row r="11" spans="1:10" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="84">
+      <c r="A11" s="95">
         <v>1</v>
       </c>
-      <c r="B11" s="82" t="s">
+      <c r="B11" s="97" t="s">
         <v>54</v>
       </c>
-      <c r="C11" s="55" t="s">
+      <c r="C11" s="48" t="s">
         <v>61</v>
       </c>
       <c r="D11" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="E11" s="70"/>
-      <c r="F11" s="38" t="s">
+      <c r="E11" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="F11" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="G11" s="70"/>
-      <c r="H11" s="72" t="s">
+      <c r="G11" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="H11" s="61" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="12" spans="1:10" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="85"/>
-      <c r="B12" s="83"/>
-      <c r="C12" s="57" t="s">
+      <c r="A12" s="96"/>
+      <c r="B12" s="98"/>
+      <c r="C12" s="50" t="s">
         <v>62</v>
       </c>
       <c r="D12" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="E12" s="71"/>
-      <c r="F12" s="38" t="s">
+      <c r="E12" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="F12" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="G12" s="44"/>
-      <c r="H12" s="72" t="s">
+      <c r="G12" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="H12" s="61" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:10" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="85"/>
-      <c r="B13" s="83"/>
-      <c r="C13" s="51" t="s">
+      <c r="A13" s="96"/>
+      <c r="B13" s="98"/>
+      <c r="C13" s="44" t="s">
         <v>63</v>
       </c>
       <c r="D13" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="E13" s="57"/>
-      <c r="F13" s="38" t="s">
+      <c r="E13" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="F13" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="G13" s="57"/>
-      <c r="H13" s="72" t="s">
+      <c r="G13" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="H13" s="61" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:10" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="85"/>
-      <c r="B14" s="83"/>
-      <c r="C14" s="55" t="s">
+      <c r="A14" s="96"/>
+      <c r="B14" s="98"/>
+      <c r="C14" s="48" t="s">
         <v>58</v>
       </c>
       <c r="D14" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="E14" s="70"/>
-      <c r="F14" s="38" t="s">
+      <c r="E14" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="F14" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="G14" s="70"/>
-      <c r="H14" s="72" t="s">
+      <c r="G14" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="H14" s="61" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:10" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="85"/>
-      <c r="B15" s="83"/>
-      <c r="C15" s="57" t="s">
+      <c r="A15" s="96"/>
+      <c r="B15" s="98"/>
+      <c r="C15" s="50" t="s">
         <v>59</v>
       </c>
       <c r="D15" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="E15" s="62"/>
-      <c r="F15" s="38" t="s">
+      <c r="E15" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="F15" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="G15" s="44"/>
-      <c r="H15" s="72" t="s">
+      <c r="G15" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="H15" s="61" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:10" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="85"/>
-      <c r="B16" s="93"/>
-      <c r="C16" s="48" t="s">
+      <c r="A16" s="96"/>
+      <c r="B16" s="99"/>
+      <c r="C16" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="D16" s="66" t="s">
+      <c r="D16" s="58" t="s">
         <v>70</v>
       </c>
-      <c r="E16" s="69"/>
-      <c r="F16" s="63" t="s">
+      <c r="E16" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="F16" s="55" t="s">
         <v>52</v>
       </c>
-      <c r="G16" s="51"/>
-      <c r="H16" s="73" t="s">
+      <c r="G16" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="H16" s="62" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:8" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="64">
+      <c r="A17" s="56">
         <v>2</v>
       </c>
-      <c r="B17" s="60" t="s">
+      <c r="B17" s="53" t="s">
         <v>55</v>
       </c>
-      <c r="C17" s="56" t="s">
+      <c r="C17" s="49" t="s">
         <v>72</v>
       </c>
-      <c r="D17" s="65" t="s">
+      <c r="D17" s="57" t="s">
         <v>100</v>
       </c>
-      <c r="E17" s="28"/>
-      <c r="F17" s="27" t="s">
+      <c r="E17" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="F17" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="G17" s="28"/>
-      <c r="H17" s="72" t="s">
+      <c r="G17" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="H17" s="61" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="18" spans="1:8" s="19" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="75">
+      <c r="A18" s="64">
         <v>3</v>
       </c>
-      <c r="B18" s="74" t="s">
+      <c r="B18" s="63" t="s">
         <v>56</v>
       </c>
-      <c r="C18" s="67" t="s">
+      <c r="C18" s="59" t="s">
         <v>69</v>
       </c>
-      <c r="D18" s="68" t="s">
+      <c r="D18" s="60" t="s">
         <v>71</v>
       </c>
-      <c r="E18" s="67"/>
-      <c r="F18" s="38" t="s">
+      <c r="E18" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="F18" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="G18" s="67"/>
-      <c r="H18" s="72" t="s">
+      <c r="G18" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="H18" s="61" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="19" spans="1:8" s="19" customFormat="1" ht="27" x14ac:dyDescent="0.15">
-      <c r="A19" s="64">
+      <c r="A19" s="56">
         <v>4</v>
       </c>
-      <c r="B19" s="59" t="s">
+      <c r="B19" s="52" t="s">
         <v>75</v>
       </c>
-      <c r="C19" s="61" t="s">
+      <c r="C19" s="54" t="s">
         <v>102</v>
       </c>
-      <c r="D19" s="66" t="s">
+      <c r="D19" s="58" t="s">
         <v>101</v>
       </c>
-      <c r="E19" s="61"/>
-      <c r="F19" s="63" t="s">
+      <c r="E19" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="F19" s="55" t="s">
         <v>52</v>
       </c>
-      <c r="G19" s="61"/>
-      <c r="H19" s="72" t="s">
+      <c r="G19" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="H19" s="61" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="64">
+      <c r="A20" s="56">
         <v>5</v>
       </c>
-      <c r="B20" s="58" t="s">
+      <c r="B20" s="51" t="s">
         <v>57</v>
       </c>
-      <c r="C20" s="61" t="s">
+      <c r="C20" s="54" t="s">
         <v>73</v>
       </c>
-      <c r="D20" s="66" t="s">
+      <c r="D20" s="58" t="s">
         <v>74</v>
       </c>
-      <c r="E20" s="61"/>
-      <c r="F20" s="38" t="s">
+      <c r="E20" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="F20" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="G20" s="61"/>
-      <c r="H20" s="72" t="s">
+      <c r="G20" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="H20" s="61" t="s">
         <v>76</v>
       </c>
     </row>
@@ -2500,6 +2482,14 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A11:A16"/>
+    <mergeCell ref="B11:B16"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:F4"/>
     <mergeCell ref="G9:G10"/>
     <mergeCell ref="H9:H10"/>
     <mergeCell ref="A5:B6"/>
@@ -2513,14 +2503,6 @@
     <mergeCell ref="D9:D10"/>
     <mergeCell ref="E9:E10"/>
     <mergeCell ref="F9:F10"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="A11:A16"/>
-    <mergeCell ref="B11:B16"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.31496062992125984" right="0.27559055118110237" top="0.78740157480314965" bottom="0.47244094488188981" header="0.51181102362204722" footer="0.19685039370078741"/>
@@ -2538,7 +2520,7 @@
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScale="110" zoomScaleNormal="115" zoomScaleSheetLayoutView="110" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="G12" sqref="G12:G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2556,108 +2538,108 @@
   <sheetData>
     <row r="1" spans="1:10" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="86" t="s">
+      <c r="A2" s="88" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="87"/>
-      <c r="C2" s="88" t="s">
+      <c r="B2" s="89"/>
+      <c r="C2" s="90" t="s">
         <v>77</v>
       </c>
-      <c r="D2" s="88"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="88"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
       <c r="J2" s="6"/>
     </row>
     <row r="3" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="89" t="s">
+      <c r="A3" s="91" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="90"/>
-      <c r="C3" s="91" t="s">
+      <c r="B3" s="92"/>
+      <c r="C3" s="93" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="91"/>
-      <c r="E3" s="91"/>
-      <c r="F3" s="91"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="93"/>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
     </row>
     <row r="4" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="89" t="s">
+      <c r="A4" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="90"/>
-      <c r="C4" s="92" t="s">
+      <c r="B4" s="92"/>
+      <c r="C4" s="94" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="92"/>
-      <c r="E4" s="92"/>
-      <c r="F4" s="92"/>
+      <c r="D4" s="94"/>
+      <c r="E4" s="94"/>
+      <c r="F4" s="94"/>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
     </row>
     <row r="5" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="98" t="s">
+      <c r="A5" s="76" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="99"/>
-      <c r="C5" s="102" t="s">
+      <c r="B5" s="77"/>
+      <c r="C5" s="80" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="102"/>
-      <c r="E5" s="102"/>
-      <c r="F5" s="102"/>
+      <c r="D5" s="80"/>
+      <c r="E5" s="80"/>
+      <c r="F5" s="80"/>
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
     </row>
     <row r="6" spans="1:10" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="112"/>
-      <c r="B6" s="113"/>
-      <c r="C6" s="114" t="s">
+      <c r="A6" s="104"/>
+      <c r="B6" s="105"/>
+      <c r="C6" s="106" t="s">
         <v>38</v>
       </c>
-      <c r="D6" s="115"/>
-      <c r="E6" s="115"/>
-      <c r="F6" s="116"/>
+      <c r="D6" s="107"/>
+      <c r="E6" s="107"/>
+      <c r="F6" s="108"/>
       <c r="G6" s="16"/>
       <c r="H6" s="16"/>
       <c r="I6" s="14"/>
       <c r="J6" s="14"/>
     </row>
     <row r="7" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="100"/>
-      <c r="B7" s="101"/>
-      <c r="C7" s="103" t="s">
+      <c r="A7" s="78"/>
+      <c r="B7" s="79"/>
+      <c r="C7" s="81" t="s">
         <v>39</v>
       </c>
-      <c r="D7" s="103"/>
-      <c r="E7" s="103"/>
-      <c r="F7" s="103"/>
+      <c r="D7" s="81"/>
+      <c r="E7" s="81"/>
+      <c r="F7" s="81"/>
       <c r="G7" s="8"/>
       <c r="H7" s="8"/>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
     </row>
     <row r="8" spans="1:10" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="104" t="s">
+      <c r="A8" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="105"/>
-      <c r="C8" s="106" t="s">
+      <c r="B8" s="83"/>
+      <c r="C8" s="84" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="106"/>
-      <c r="E8" s="106"/>
-      <c r="F8" s="106"/>
+      <c r="D8" s="84"/>
+      <c r="E8" s="84"/>
+      <c r="F8" s="84"/>
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
       <c r="I8" s="6"/>
@@ -2665,132 +2647,148 @@
     </row>
     <row r="9" spans="1:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="10" spans="1:10" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="107" t="s">
+      <c r="A10" s="85" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="108" t="s">
+      <c r="B10" s="86" t="s">
         <v>48</v>
       </c>
-      <c r="C10" s="94" t="s">
+      <c r="C10" s="72" t="s">
         <v>44</v>
       </c>
-      <c r="D10" s="94" t="s">
+      <c r="D10" s="72" t="s">
         <v>46</v>
       </c>
-      <c r="E10" s="94" t="s">
+      <c r="E10" s="72" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="94" t="s">
+      <c r="F10" s="72" t="s">
         <v>42</v>
       </c>
-      <c r="G10" s="94" t="s">
+      <c r="G10" s="72" t="s">
         <v>40</v>
       </c>
-      <c r="H10" s="110" t="s">
+      <c r="H10" s="109" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="100"/>
-      <c r="B11" s="109"/>
-      <c r="C11" s="95"/>
-      <c r="D11" s="95"/>
-      <c r="E11" s="95"/>
-      <c r="F11" s="95"/>
-      <c r="G11" s="95"/>
-      <c r="H11" s="111"/>
+      <c r="A11" s="78"/>
+      <c r="B11" s="87"/>
+      <c r="C11" s="73"/>
+      <c r="D11" s="73"/>
+      <c r="E11" s="73"/>
+      <c r="F11" s="73"/>
+      <c r="G11" s="73"/>
+      <c r="H11" s="110"/>
     </row>
     <row r="12" spans="1:10" s="3" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="117">
+      <c r="A12" s="100">
         <v>1</v>
       </c>
-      <c r="B12" s="82" t="s">
+      <c r="B12" s="97" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="119" t="s">
+      <c r="C12" s="102" t="s">
         <v>50</v>
       </c>
-      <c r="D12" s="45" t="s">
+      <c r="D12" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="E12" s="38"/>
-      <c r="F12" s="38" t="s">
+      <c r="E12" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="F12" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="G12" s="38"/>
-      <c r="H12" s="52" t="s">
+      <c r="G12" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="H12" s="45" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:10" s="13" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="118"/>
-      <c r="B13" s="93"/>
-      <c r="C13" s="120"/>
-      <c r="D13" s="48" t="s">
+      <c r="A13" s="101"/>
+      <c r="B13" s="99"/>
+      <c r="C13" s="103"/>
+      <c r="D13" s="41" t="s">
         <v>103</v>
       </c>
-      <c r="E13" s="40"/>
-      <c r="F13" s="38" t="s">
+      <c r="E13" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="F13" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="G13" s="40"/>
-      <c r="H13" s="52" t="s">
+      <c r="G13" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="H13" s="45" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:10" s="13" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="26">
+      <c r="A14" s="23">
         <v>2</v>
       </c>
-      <c r="B14" s="50" t="s">
+      <c r="B14" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="28" t="s">
+      <c r="C14" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="D14" s="28" t="s">
+      <c r="D14" s="25" t="s">
         <v>82</v>
       </c>
-      <c r="E14" s="28"/>
-      <c r="F14" s="38" t="s">
+      <c r="E14" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="F14" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="G14" s="27"/>
-      <c r="H14" s="52" t="s">
+      <c r="G14" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="H14" s="45" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:10" s="3" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="26">
+      <c r="A15" s="23">
         <v>3</v>
       </c>
-      <c r="B15" s="50" t="s">
+      <c r="B15" s="43" t="s">
         <v>83</v>
       </c>
-      <c r="C15" s="28" t="s">
+      <c r="C15" s="25" t="s">
         <v>84</v>
       </c>
-      <c r="D15" s="28" t="s">
+      <c r="D15" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="E15" s="28"/>
-      <c r="F15" s="38" t="s">
+      <c r="E15" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="F15" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="G15" s="27"/>
-      <c r="H15" s="52" t="s">
+      <c r="G15" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="H15" s="45" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:10" s="13" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="21"/>
-      <c r="B16" s="140"/>
+      <c r="B16" s="70"/>
       <c r="C16" s="20"/>
       <c r="D16" s="20"/>
       <c r="E16" s="20"/>
       <c r="F16" s="21"/>
       <c r="G16" s="21"/>
-      <c r="H16" s="141"/>
+      <c r="H16" s="71"/>
     </row>
     <row r="17" spans="1:8" s="3" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="4"/>
@@ -2848,29 +2846,29 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="A5:B7"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C6:F6"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="C10:C11"/>
-    <mergeCell ref="A5:B7"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="G10:G11"/>
-    <mergeCell ref="H10:H11"/>
-    <mergeCell ref="F10:F11"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.31496062992125984" right="0.27559055118110237" top="0.78740157480314965" bottom="0.47244094488188981" header="0.51181102362204722" footer="0.19685039370078741"/>
@@ -2886,8 +2884,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A22" zoomScale="110" zoomScaleNormal="85" zoomScaleSheetLayoutView="110" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A11" zoomScale="110" zoomScaleNormal="85" zoomScaleSheetLayoutView="110" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12:G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2905,108 +2903,108 @@
   <sheetData>
     <row r="1" spans="1:10" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="86" t="s">
+      <c r="A2" s="88" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="87"/>
-      <c r="C2" s="88" t="s">
+      <c r="B2" s="89"/>
+      <c r="C2" s="90" t="s">
         <v>77</v>
       </c>
-      <c r="D2" s="88"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="88"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="90"/>
+      <c r="F2" s="90"/>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
       <c r="I2" s="6"/>
       <c r="J2" s="6"/>
     </row>
     <row r="3" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="89" t="s">
+      <c r="A3" s="91" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="90"/>
-      <c r="C3" s="91" t="s">
+      <c r="B3" s="92"/>
+      <c r="C3" s="93" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="91"/>
-      <c r="E3" s="91"/>
-      <c r="F3" s="91"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="93"/>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
     </row>
     <row r="4" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="89" t="s">
+      <c r="A4" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="90"/>
-      <c r="C4" s="92" t="s">
+      <c r="B4" s="92"/>
+      <c r="C4" s="94" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="92"/>
-      <c r="E4" s="92"/>
-      <c r="F4" s="92"/>
+      <c r="D4" s="94"/>
+      <c r="E4" s="94"/>
+      <c r="F4" s="94"/>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
     </row>
     <row r="5" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="89" t="s">
+      <c r="A5" s="91" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="90"/>
-      <c r="C5" s="102" t="s">
+      <c r="B5" s="92"/>
+      <c r="C5" s="80" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="102"/>
-      <c r="E5" s="102"/>
-      <c r="F5" s="102"/>
+      <c r="D5" s="80"/>
+      <c r="E5" s="80"/>
+      <c r="F5" s="80"/>
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
     </row>
     <row r="6" spans="1:10" s="9" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="89"/>
-      <c r="B6" s="90"/>
-      <c r="C6" s="128" t="s">
+      <c r="A6" s="91"/>
+      <c r="B6" s="92"/>
+      <c r="C6" s="118" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="129"/>
-      <c r="E6" s="129"/>
-      <c r="F6" s="130"/>
+      <c r="D6" s="119"/>
+      <c r="E6" s="119"/>
+      <c r="F6" s="120"/>
       <c r="G6" s="11"/>
       <c r="H6" s="11"/>
       <c r="I6" s="10"/>
       <c r="J6" s="10"/>
     </row>
     <row r="7" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="89"/>
-      <c r="B7" s="90"/>
-      <c r="C7" s="103" t="s">
+      <c r="A7" s="91"/>
+      <c r="B7" s="92"/>
+      <c r="C7" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="103"/>
-      <c r="E7" s="103"/>
-      <c r="F7" s="103"/>
+      <c r="D7" s="81"/>
+      <c r="E7" s="81"/>
+      <c r="F7" s="81"/>
       <c r="G7" s="8"/>
       <c r="H7" s="8"/>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
     </row>
     <row r="8" spans="1:10" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="131" t="s">
+      <c r="A8" s="121" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="132"/>
-      <c r="C8" s="106" t="s">
+      <c r="B8" s="122"/>
+      <c r="C8" s="84" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="106"/>
-      <c r="E8" s="106"/>
-      <c r="F8" s="106"/>
+      <c r="D8" s="84"/>
+      <c r="E8" s="84"/>
+      <c r="F8" s="84"/>
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
       <c r="I8" s="6"/>
@@ -3014,339 +3012,413 @@
     </row>
     <row r="9" spans="1:10" ht="14.25" thickBot="1" x14ac:dyDescent="0.2"/>
     <row r="10" spans="1:10" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="107" t="s">
+      <c r="A10" s="85" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="108" t="s">
+      <c r="B10" s="86" t="s">
         <v>49</v>
       </c>
-      <c r="C10" s="94" t="s">
+      <c r="C10" s="72" t="s">
         <v>45</v>
       </c>
-      <c r="D10" s="94" t="s">
+      <c r="D10" s="72" t="s">
         <v>47</v>
       </c>
-      <c r="E10" s="94" t="s">
+      <c r="E10" s="72" t="s">
         <v>15</v>
       </c>
-      <c r="F10" s="94" t="s">
+      <c r="F10" s="72" t="s">
         <v>43</v>
       </c>
-      <c r="G10" s="94" t="s">
+      <c r="G10" s="72" t="s">
         <v>41</v>
       </c>
-      <c r="H10" s="94" t="s">
+      <c r="H10" s="72" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="100"/>
-      <c r="B11" s="109"/>
-      <c r="C11" s="95"/>
-      <c r="D11" s="95"/>
-      <c r="E11" s="95"/>
-      <c r="F11" s="95"/>
-      <c r="G11" s="95"/>
-      <c r="H11" s="109"/>
+      <c r="A11" s="78"/>
+      <c r="B11" s="87"/>
+      <c r="C11" s="73"/>
+      <c r="D11" s="73"/>
+      <c r="E11" s="73"/>
+      <c r="F11" s="73"/>
+      <c r="G11" s="73"/>
+      <c r="H11" s="87"/>
     </row>
     <row r="12" spans="1:10" s="3" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="137">
+      <c r="A12" s="116">
         <v>1</v>
       </c>
-      <c r="B12" s="83" t="s">
+      <c r="B12" s="98" t="s">
         <v>88</v>
       </c>
-      <c r="C12" s="45" t="s">
+      <c r="C12" s="38" t="s">
         <v>93</v>
       </c>
-      <c r="D12" s="45" t="s">
+      <c r="D12" s="38" t="s">
         <v>90</v>
       </c>
-      <c r="E12" s="23"/>
-      <c r="F12" s="41" t="s">
+      <c r="E12" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="F12" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="G12" s="38"/>
-      <c r="H12" s="119" t="s">
+      <c r="G12" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="H12" s="102" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:10" s="3" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="137"/>
-      <c r="B13" s="82"/>
-      <c r="C13" s="46" t="s">
+      <c r="A13" s="116"/>
+      <c r="B13" s="97"/>
+      <c r="C13" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="46" t="s">
+      <c r="D13" s="39" t="s">
         <v>92</v>
       </c>
-      <c r="E13" s="22"/>
-      <c r="F13" s="53" t="s">
+      <c r="E13" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="F13" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="G13" s="39"/>
-      <c r="H13" s="119"/>
+      <c r="G13" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="H13" s="102"/>
     </row>
     <row r="14" spans="1:10" s="13" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="137"/>
-      <c r="B14" s="93"/>
-      <c r="C14" s="48" t="s">
+      <c r="A14" s="116"/>
+      <c r="B14" s="99"/>
+      <c r="C14" s="41" t="s">
         <v>94</v>
       </c>
-      <c r="D14" s="48" t="s">
+      <c r="D14" s="41" t="s">
         <v>95</v>
       </c>
-      <c r="E14" s="25"/>
-      <c r="F14" s="54" t="s">
+      <c r="E14" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="F14" s="47" t="s">
         <v>52</v>
       </c>
-      <c r="G14" s="40"/>
-      <c r="H14" s="120"/>
+      <c r="G14" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="H14" s="103"/>
     </row>
     <row r="15" spans="1:10" s="13" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="137"/>
-      <c r="B15" s="83" t="s">
+      <c r="A15" s="116"/>
+      <c r="B15" s="98" t="s">
         <v>89</v>
       </c>
-      <c r="C15" s="80" t="s">
+      <c r="C15" s="68" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="80" t="s">
+      <c r="D15" s="68" t="s">
         <v>91</v>
       </c>
-      <c r="E15" s="38"/>
-      <c r="F15" s="78" t="s">
+      <c r="E15" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="F15" s="67" t="s">
         <v>52</v>
       </c>
-      <c r="G15" s="38"/>
-      <c r="H15" s="119" t="s">
+      <c r="G15" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="H15" s="102" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="16" spans="1:10" s="13" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="137"/>
-      <c r="B16" s="83"/>
-      <c r="C16" s="81" t="s">
+      <c r="A16" s="116"/>
+      <c r="B16" s="98"/>
+      <c r="C16" s="69" t="s">
         <v>33</v>
       </c>
-      <c r="D16" s="81" t="s">
+      <c r="D16" s="69" t="s">
         <v>96</v>
       </c>
-      <c r="E16" s="39"/>
-      <c r="F16" s="78" t="s">
+      <c r="E16" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="F16" s="67" t="s">
         <v>52</v>
       </c>
-      <c r="G16" s="39"/>
-      <c r="H16" s="122"/>
+      <c r="G16" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="H16" s="114"/>
     </row>
     <row r="17" spans="1:8" s="13" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="137"/>
-      <c r="B17" s="93"/>
-      <c r="C17" s="48" t="s">
+      <c r="A17" s="116"/>
+      <c r="B17" s="99"/>
+      <c r="C17" s="41" t="s">
         <v>94</v>
       </c>
-      <c r="D17" s="48" t="s">
+      <c r="D17" s="41" t="s">
         <v>104</v>
       </c>
-      <c r="E17" s="40"/>
-      <c r="F17" s="78" t="s">
+      <c r="E17" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="F17" s="67" t="s">
         <v>52</v>
       </c>
-      <c r="G17" s="40"/>
-      <c r="H17" s="120"/>
+      <c r="G17" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="H17" s="103"/>
     </row>
     <row r="18" spans="1:8" s="13" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="137"/>
-      <c r="B18" s="76" t="s">
+      <c r="A18" s="116"/>
+      <c r="B18" s="65" t="s">
         <v>113</v>
       </c>
-      <c r="C18" s="77" t="s">
+      <c r="C18" s="66" t="s">
         <v>114</v>
       </c>
-      <c r="D18" s="77" t="s">
+      <c r="D18" s="66" t="s">
         <v>115</v>
       </c>
-      <c r="E18" s="79"/>
-      <c r="F18" s="78" t="s">
+      <c r="E18" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="F18" s="67" t="s">
         <v>112</v>
       </c>
-      <c r="G18" s="79"/>
-      <c r="H18" s="28" t="s">
+      <c r="G18" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="H18" s="25" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="19" spans="1:8" s="13" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="137"/>
-      <c r="B19" s="76" t="s">
+      <c r="A19" s="116"/>
+      <c r="B19" s="65" t="s">
         <v>109</v>
       </c>
-      <c r="C19" s="77" t="s">
+      <c r="C19" s="66" t="s">
         <v>110</v>
       </c>
-      <c r="D19" s="77" t="s">
+      <c r="D19" s="66" t="s">
         <v>111</v>
       </c>
-      <c r="E19" s="79"/>
-      <c r="F19" s="78" t="s">
+      <c r="E19" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="F19" s="67" t="s">
         <v>112</v>
       </c>
-      <c r="G19" s="79"/>
-      <c r="H19" s="28" t="s">
+      <c r="G19" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="H19" s="25" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:8" s="3" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="137"/>
-      <c r="B20" s="50" t="s">
+      <c r="A20" s="116"/>
+      <c r="B20" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="28" t="s">
+      <c r="C20" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="D20" s="28" t="s">
+      <c r="D20" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="E20" s="28"/>
-      <c r="F20" s="54" t="s">
+      <c r="E20" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="F20" s="47" t="s">
         <v>52</v>
       </c>
-      <c r="G20" s="27"/>
-      <c r="H20" s="28" t="s">
+      <c r="G20" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="H20" s="25" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:8" s="13" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="137"/>
-      <c r="B21" s="82" t="s">
+      <c r="A21" s="116"/>
+      <c r="B21" s="97" t="s">
         <v>29</v>
       </c>
-      <c r="C21" s="45" t="s">
+      <c r="C21" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="D21" s="119" t="s">
+      <c r="D21" s="102" t="s">
         <v>98</v>
       </c>
-      <c r="E21" s="125"/>
-      <c r="F21" s="127" t="s">
+      <c r="E21" s="126" t="s">
+        <v>116</v>
+      </c>
+      <c r="F21" s="128" t="s">
         <v>51</v>
       </c>
-      <c r="G21" s="125"/>
-      <c r="H21" s="119" t="s">
+      <c r="G21" s="126" t="s">
+        <v>116</v>
+      </c>
+      <c r="H21" s="102" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="22" spans="1:8" s="13" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="137"/>
-      <c r="B22" s="83"/>
-      <c r="C22" s="46" t="s">
+      <c r="A22" s="116"/>
+      <c r="B22" s="98"/>
+      <c r="C22" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="D22" s="121"/>
-      <c r="E22" s="126"/>
-      <c r="F22" s="123"/>
-      <c r="G22" s="126"/>
-      <c r="H22" s="123"/>
+      <c r="D22" s="123"/>
+      <c r="E22" s="127"/>
+      <c r="F22" s="124"/>
+      <c r="G22" s="127"/>
+      <c r="H22" s="124"/>
     </row>
     <row r="23" spans="1:8" s="13" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="137"/>
-      <c r="B23" s="93"/>
-      <c r="C23" s="48" t="s">
+      <c r="A23" s="116"/>
+      <c r="B23" s="99"/>
+      <c r="C23" s="41" t="s">
         <v>97</v>
       </c>
-      <c r="D23" s="48" t="s">
+      <c r="D23" s="41" t="s">
         <v>99</v>
       </c>
-      <c r="E23" s="24"/>
-      <c r="F23" s="54" t="s">
+      <c r="E23" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="F23" s="47" t="s">
         <v>52</v>
       </c>
-      <c r="G23" s="42"/>
-      <c r="H23" s="124"/>
+      <c r="G23" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="H23" s="125"/>
     </row>
     <row r="24" spans="1:8" s="12" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="117">
+      <c r="A24" s="100">
         <v>2</v>
       </c>
-      <c r="B24" s="119" t="s">
+      <c r="B24" s="102" t="s">
         <v>31</v>
       </c>
-      <c r="C24" s="45" t="s">
+      <c r="C24" s="38" t="s">
         <v>105</v>
       </c>
-      <c r="D24" s="119" t="s">
+      <c r="D24" s="102" t="s">
         <v>35</v>
       </c>
-      <c r="E24" s="119"/>
-      <c r="F24" s="119" t="s">
+      <c r="E24" s="102" t="s">
+        <v>116</v>
+      </c>
+      <c r="F24" s="102" t="s">
         <v>51</v>
       </c>
-      <c r="G24" s="139"/>
-      <c r="H24" s="133" t="s">
+      <c r="G24" s="102" t="s">
+        <v>116</v>
+      </c>
+      <c r="H24" s="111" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="25" spans="1:8" s="12" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="137"/>
-      <c r="B25" s="122"/>
-      <c r="C25" s="47" t="s">
+      <c r="A25" s="116"/>
+      <c r="B25" s="114"/>
+      <c r="C25" s="40" t="s">
         <v>106</v>
       </c>
-      <c r="D25" s="122"/>
-      <c r="E25" s="122"/>
-      <c r="F25" s="122"/>
-      <c r="G25" s="134"/>
-      <c r="H25" s="134"/>
+      <c r="D25" s="114"/>
+      <c r="E25" s="114"/>
+      <c r="F25" s="114"/>
+      <c r="G25" s="114"/>
+      <c r="H25" s="112"/>
     </row>
     <row r="26" spans="1:8" ht="50.1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="137"/>
-      <c r="B26" s="122"/>
-      <c r="C26" s="47" t="s">
+      <c r="A26" s="116"/>
+      <c r="B26" s="114"/>
+      <c r="C26" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="D26" s="122"/>
-      <c r="E26" s="122"/>
-      <c r="F26" s="122"/>
-      <c r="G26" s="134"/>
-      <c r="H26" s="134"/>
+      <c r="D26" s="114"/>
+      <c r="E26" s="114"/>
+      <c r="F26" s="114"/>
+      <c r="G26" s="114"/>
+      <c r="H26" s="112"/>
     </row>
     <row r="27" spans="1:8" s="12" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="137"/>
-      <c r="B27" s="122"/>
-      <c r="C27" s="51" t="s">
+      <c r="A27" s="116"/>
+      <c r="B27" s="114"/>
+      <c r="C27" s="44" t="s">
         <v>107</v>
       </c>
-      <c r="D27" s="122"/>
-      <c r="E27" s="122"/>
-      <c r="F27" s="122"/>
-      <c r="G27" s="134"/>
-      <c r="H27" s="134"/>
+      <c r="D27" s="114"/>
+      <c r="E27" s="114"/>
+      <c r="F27" s="114"/>
+      <c r="G27" s="114"/>
+      <c r="H27" s="112"/>
     </row>
     <row r="28" spans="1:8" s="12" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="137"/>
-      <c r="B28" s="122"/>
-      <c r="C28" s="51" t="s">
+      <c r="A28" s="116"/>
+      <c r="B28" s="114"/>
+      <c r="C28" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="D28" s="122"/>
-      <c r="E28" s="122"/>
-      <c r="F28" s="122"/>
-      <c r="G28" s="134"/>
-      <c r="H28" s="134"/>
+      <c r="D28" s="114"/>
+      <c r="E28" s="114"/>
+      <c r="F28" s="114"/>
+      <c r="G28" s="114"/>
+      <c r="H28" s="112"/>
     </row>
     <row r="29" spans="1:8" s="12" customFormat="1" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="138"/>
-      <c r="B29" s="136"/>
-      <c r="C29" s="49" t="s">
+      <c r="A29" s="117"/>
+      <c r="B29" s="115"/>
+      <c r="C29" s="42" t="s">
         <v>108</v>
       </c>
-      <c r="D29" s="136"/>
-      <c r="E29" s="136"/>
-      <c r="F29" s="136"/>
-      <c r="G29" s="135"/>
-      <c r="H29" s="135"/>
+      <c r="D29" s="115"/>
+      <c r="E29" s="115"/>
+      <c r="F29" s="115"/>
+      <c r="G29" s="115"/>
+      <c r="H29" s="113"/>
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="H12:H14"/>
+    <mergeCell ref="H21:H23"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="G21:G22"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="A5:B7"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:F4"/>
     <mergeCell ref="H24:H29"/>
     <mergeCell ref="B24:B29"/>
     <mergeCell ref="A24:A29"/>
@@ -3359,32 +3431,6 @@
     <mergeCell ref="D24:D29"/>
     <mergeCell ref="B15:B17"/>
     <mergeCell ref="H15:H17"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="A5:B7"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="H10:H11"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="H12:H14"/>
-    <mergeCell ref="H21:H23"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="G21:G22"/>
-    <mergeCell ref="F21:F22"/>
-    <mergeCell ref="G10:G11"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.31496062992125984" right="0.27559055118110237" top="0.78740157480314965" bottom="0.47244094488188981" header="0.51181102362204722" footer="0.19685039370078741"/>

</xml_diff>